<commit_message>
added check_headers + unittest and fixed nested_attributes tests
</commit_message>
<xml_diff>
--- a/UnitTests/Excel/Testfiles/nested_attributes_1.xlsx
+++ b/UnitTests/Excel/Testfiles/nested_attributes_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t xml:space="preserve">typeURI</t>
   </si>
@@ -52,15 +52,9 @@
     <t xml:space="preserve">testComplexTypeMetKard[].testKwantWrd</t>
   </si>
   <si>
-    <t xml:space="preserve">testComplexTypeMetKard[].testKwantWrdMetKard[]</t>
-  </si>
-  <si>
     <t xml:space="preserve">testComplexTypeMetKard[].testStringField</t>
   </si>
   <si>
-    <t xml:space="preserve">testComplexTypeMetKard[].testStringFieldMetKard[]</t>
-  </si>
-  <si>
     <t xml:space="preserve">testUnionType.unionString</t>
   </si>
   <si>
@@ -89,9 +83,6 @@
   </si>
   <si>
     <t xml:space="preserve">True|False</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;unable to write a nested list in a csv&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">RWKofW</t>
@@ -110,6 +101,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -195,13 +187,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.4"/>
@@ -209,15 +201,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="35.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="35.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="35.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="37.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="35.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="43.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="35.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="43.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="22.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="34.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="35.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="34.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -260,58 +250,46 @@
       <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>65.14</v>
       </c>
       <c r="F2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="J2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>23</v>
       </c>
       <c r="L2" s="0" t="s">
         <v>21</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>